<commit_message>
Detect 'extra' models in gdb, update test xlsx to mimic 'extra' model
</commit_message>
<xml_diff>
--- a/TestGDBExcel.xlsx
+++ b/TestGDBExcel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="9580" windowHeight="8690"/>
+    <workbookView activeTab="0" windowWidth="8860" windowHeight="3290"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -139,8 +139,8 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0" tabSelected="1">
+      <selection activeCell="A9" sqref="A9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -302,25 +302,7 @@
         </is>
       </c>
     </row>
-    <row r="9" spans="1:5" customHeight="1" ht="19.5">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>380122</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>256</t>
-        </is>
-      </c>
-    </row>
+    <row r="9" spans="1:5" customHeight="1" ht="19.5"/>
     <row r="10" spans="1:5" customHeight="1" ht="19.5">
       <c r="A10" t="s">
         <v>6</v>
@@ -386,8 +368,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="2" width="9.142307692307693"/>
-    <col min="2" max="16384" style="2" width="9.142307692307693"/>
+    <col min="1" max="16384" style="2" width="9.142307692307693"/>
   </cols>
   <sheetData/>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>

</xml_diff>